<commit_message>
v0.48 Fixed Mode Selection Reg Write
</commit_message>
<xml_diff>
--- a/Documentation/Feedback & ToDoList/4711_GUI_FB_0.7.xlsx
+++ b/Documentation/Feedback & ToDoList/4711_GUI_FB_0.7.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="147">
   <si>
     <t>I2C Device Address加上</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -875,6 +875,14 @@
   </si>
   <si>
     <t>Done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DOne</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1022,7 +1030,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1070,6 +1078,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="3" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="差" xfId="3" builtinId="27"/>
@@ -1110,7 +1119,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1375A446-59C3-4408-9B54-31A206487CDA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1375A446-59C3-4408-9B54-31A206487CDA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1154,7 +1163,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C10189AD-A3A4-4692-9AD8-ED27FA1AD856}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C10189AD-A3A4-4692-9AD8-ED27FA1AD856}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1198,7 +1207,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5458403-52AE-49CF-B170-B077049CF2C4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D5458403-52AE-49CF-B170-B077049CF2C4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1934,8 +1943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:H86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="E25" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2174,6 +2183,9 @@
       <c r="G30" s="13" t="s">
         <v>138</v>
       </c>
+      <c r="H30" s="26" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="31" spans="4:8" ht="27">
       <c r="E31" s="9">
@@ -2185,6 +2197,9 @@
       <c r="G31" s="13" t="s">
         <v>101</v>
       </c>
+      <c r="H31" s="26" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="32" spans="4:8" ht="27">
       <c r="E32" s="9">
@@ -2196,6 +2211,9 @@
       <c r="G32" s="13" t="s">
         <v>101</v>
       </c>
+      <c r="H32" s="26" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="33" spans="4:8" s="15" customFormat="1">
       <c r="E33" s="10">
@@ -2217,7 +2235,7 @@
       </c>
     </row>
     <row r="36" spans="4:8" ht="24" customHeight="1">
-      <c r="E36" s="26">
+      <c r="E36" s="27">
         <v>2</v>
       </c>
       <c r="F36" s="10" t="s">
@@ -2225,7 +2243,7 @@
       </c>
     </row>
     <row r="37" spans="4:8" ht="108">
-      <c r="E37" s="26"/>
+      <c r="E37" s="27"/>
       <c r="F37" s="11" t="s">
         <v>99</v>
       </c>

</xml_diff>

<commit_message>
v0.49 Added EQ Download/Import/Export and VOL1/2/3/4 ...
</commit_message>
<xml_diff>
--- a/Documentation/Feedback & ToDoList/4711_GUI_FB_0.7.xlsx
+++ b/Documentation/Feedback & ToDoList/4711_GUI_FB_0.7.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="153">
   <si>
     <t>I2C Device Address加上</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -883,6 +883,30 @@
   </si>
   <si>
     <t>DOne</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fixed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>我这里无法重现</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>这个的确不更新，因为无法知道你到底读哪个，要是每次读都去判断是否需要更新到界面比较烦琐。不过要是的确需要也可以加</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Done</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1030,7 +1054,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1069,7 +1093,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1077,6 +1100,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="3" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
@@ -1523,8 +1548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1927,9 +1952,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="S70" sqref="S70"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
@@ -1943,8 +1966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:H86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E25" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="H70" sqref="H70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1975,8 +1998,8 @@
       <c r="F3" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19" t="s">
+      <c r="G3" s="18"/>
+      <c r="H3" s="18" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1987,7 +2010,7 @@
       <c r="F4" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="23" t="s">
         <v>144</v>
       </c>
     </row>
@@ -1998,12 +2021,12 @@
       <c r="F5" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="G5" s="19"/>
-      <c r="H5" s="25" t="s">
+      <c r="G5" s="18"/>
+      <c r="H5" s="24" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="3:8" s="20" customFormat="1">
+    <row r="6" spans="3:8" s="19" customFormat="1">
       <c r="F6" s="10" t="s">
         <v>137</v>
       </c>
@@ -2043,8 +2066,10 @@
       <c r="F12" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="26" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="13" spans="3:8">
       <c r="E13">
@@ -2053,21 +2078,23 @@
       <c r="F13" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="G13" s="22" t="s">
+      <c r="G13" s="21" t="s">
         <v>110</v>
       </c>
       <c r="H13" s="10" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="14" spans="3:8" s="20" customFormat="1">
-      <c r="E14" s="20">
+    <row r="14" spans="3:8" s="19" customFormat="1">
+      <c r="E14" s="19">
         <v>3</v>
       </c>
       <c r="F14" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="G14" s="18"/>
+      <c r="G14" s="26" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="17" spans="4:8">
       <c r="D17" t="s">
@@ -2095,7 +2122,7 @@
       <c r="F19" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="H19" s="19" t="s">
+      <c r="H19" s="18" t="s">
         <v>129</v>
       </c>
     </row>
@@ -2109,7 +2136,7 @@
       <c r="F21" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="H21" s="19" t="s">
+      <c r="H21" s="18" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2140,10 +2167,10 @@
       <c r="F25" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="G25" s="19" t="s">
+      <c r="G25" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="H25" s="23" t="s">
+      <c r="H25" s="22" t="s">
         <v>143</v>
       </c>
     </row>
@@ -2166,6 +2193,9 @@
       <c r="F28" s="10" t="s">
         <v>105</v>
       </c>
+      <c r="G28" s="26" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="29" spans="4:8">
       <c r="F29" s="7"/>
@@ -2183,7 +2213,7 @@
       <c r="G30" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="H30" s="26" t="s">
+      <c r="H30" s="25" t="s">
         <v>145</v>
       </c>
     </row>
@@ -2197,7 +2227,7 @@
       <c r="G31" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="H31" s="26" t="s">
+      <c r="H31" s="25" t="s">
         <v>146</v>
       </c>
     </row>
@@ -2211,7 +2241,7 @@
       <c r="G32" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="H32" s="26" t="s">
+      <c r="H32" s="25" t="s">
         <v>146</v>
       </c>
     </row>
@@ -2235,7 +2265,7 @@
       </c>
     </row>
     <row r="36" spans="4:8" ht="24" customHeight="1">
-      <c r="E36" s="27">
+      <c r="E36" s="28">
         <v>2</v>
       </c>
       <c r="F36" s="10" t="s">
@@ -2243,9 +2273,12 @@
       </c>
     </row>
     <row r="37" spans="4:8" ht="108">
-      <c r="E37" s="27"/>
+      <c r="E37" s="28"/>
       <c r="F37" s="11" t="s">
         <v>99</v>
+      </c>
+      <c r="H37" s="26" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="39" spans="4:8">
@@ -2259,18 +2292,18 @@
         <v>91</v>
       </c>
     </row>
-    <row r="41" spans="4:8" s="21" customFormat="1">
-      <c r="D41" s="21" t="s">
+    <row r="41" spans="4:8" s="20" customFormat="1">
+      <c r="D41" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="E41" s="21">
+      <c r="E41" s="20">
         <v>1</v>
       </c>
-      <c r="F41" s="21" t="s">
+      <c r="F41" s="20" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="42" spans="4:8" s="21" customFormat="1"/>
+    <row r="42" spans="4:8" s="20" customFormat="1"/>
     <row r="43" spans="4:8">
       <c r="D43" s="10" t="s">
         <v>62</v>
@@ -2281,8 +2314,11 @@
       <c r="F43" s="10" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="44" spans="4:8" s="21" customFormat="1">
+      <c r="H43" s="26" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="44" spans="4:8" s="20" customFormat="1">
       <c r="D44" s="10"/>
       <c r="E44" s="10">
         <v>2</v>
@@ -2290,7 +2326,7 @@
       <c r="F44" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="H44" s="23" t="s">
+      <c r="H44" s="22" t="s">
         <v>143</v>
       </c>
     </row>
@@ -2302,6 +2338,9 @@
       <c r="F46" s="10" t="s">
         <v>65</v>
       </c>
+      <c r="H46" s="26" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="48" spans="4:8">
       <c r="D48" t="s">
@@ -2321,7 +2360,7 @@
       <c r="F50" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="H50" s="19" t="s">
+      <c r="H50" s="18" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2357,7 +2396,7 @@
       <c r="F56" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="H56" s="19" t="s">
+      <c r="H56" s="18" t="s">
         <v>131</v>
       </c>
     </row>
@@ -2368,7 +2407,7 @@
       <c r="F57" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="H57" s="19" t="s">
+      <c r="H57" s="18" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2378,6 +2417,9 @@
       </c>
       <c r="F59" s="10" t="s">
         <v>76</v>
+      </c>
+      <c r="H59" s="27" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="60" spans="3:8">
@@ -2395,7 +2437,7 @@
       <c r="F62" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="G62" s="19" t="s">
+      <c r="G62" s="18" t="s">
         <v>133</v>
       </c>
     </row>
@@ -2417,7 +2459,7 @@
       <c r="F65" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="H65" s="19" t="s">
+      <c r="H65" s="18" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2440,6 +2482,9 @@
       <c r="F68" s="10" t="s">
         <v>82</v>
       </c>
+      <c r="H68" s="27" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="69" spans="4:8">
       <c r="D69" s="10"/>
@@ -2449,6 +2494,9 @@
       <c r="F69" s="10" t="s">
         <v>98</v>
       </c>
+      <c r="H69" s="27" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="70" spans="4:8">
       <c r="D70" s="10"/>
@@ -2458,6 +2506,9 @@
       <c r="F70" s="10" t="s">
         <v>97</v>
       </c>
+      <c r="H70" s="27" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="71" spans="4:8">
       <c r="D71" s="10"/>
@@ -2502,10 +2553,10 @@
       </c>
     </row>
     <row r="78" spans="4:8">
-      <c r="D78" s="20" t="s">
+      <c r="D78" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="E78" s="20">
+      <c r="E78" s="19">
         <v>1</v>
       </c>
       <c r="F78" s="9" t="s">
@@ -2519,7 +2570,7 @@
       <c r="F79" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="H79" s="19" t="s">
+      <c r="H79" s="18" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2530,7 +2581,7 @@
       <c r="F80" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="H80" s="19" t="s">
+      <c r="H80" s="18" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2541,7 +2592,7 @@
       <c r="F81" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="H81" s="19" t="s">
+      <c r="H81" s="18" t="s">
         <v>134</v>
       </c>
     </row>

</xml_diff>